<commit_message>
31/02/23 1. Update Setup Portofolio, Setup Kegiatan, and Setup Klasifikasi 2. Scripting Setup Fund Manager, Setup Custodian 3. Scripting DPLKKEU009-001 and DPLKKEU010-001
01/02/23
1. Scripting Setup Jenis Broker, Setup Broker, DPLKINV133-001, DPLKINV135-001, DPLKKPS129-001, and DPLKKPS130-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-001 - Setup Portofolio Investasi - General Tambah.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-001 - Setup Portofolio Investasi - General Tambah.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280BBF20-2218-4EB8-BDF6-316DACEE1FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD59132-DB55-4A71-98A9-8678E36579BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DPLKINV001" sheetId="2" r:id="rId1"/>
+    <sheet name="DPLKINV001-001" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -546,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="99" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>